<commit_message>
seamless world option for ship
</commit_message>
<xml_diff>
--- a/Assets/excel/config.xlsx
+++ b/Assets/excel/config.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>key</t>
   </si>
@@ -69,6 +69,15 @@
   </si>
   <si>
     <t>Отключить трение</t>
+  </si>
+  <si>
+    <t>opt_seamless_world</t>
+  </si>
+  <si>
+    <t>Seamless world</t>
+  </si>
+  <si>
+    <t>Бесшовный мир</t>
   </si>
   <si>
     <t>help_control</t>
@@ -369,10 +378,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -449,25 +458,25 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -541,32 +550,32 @@
       <c r="A15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="0"/>
-      <c r="C15" s="0"/>
+      <c r="B15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0"/>
+      <c r="C16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>49</v>
       </c>
@@ -577,7 +586,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>52</v>
       </c>
@@ -588,7 +597,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>55</v>
       </c>
@@ -621,7 +630,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>64</v>
       </c>
@@ -632,7 +641,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>67</v>
       </c>
@@ -641,6 +650,17 @@
       </c>
       <c r="C24" s="2" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
skill radar, forgoted files from resonator commit
</commit_message>
<xml_diff>
--- a/Assets/excel/config.xlsx
+++ b/Assets/excel/config.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t>key</t>
   </si>
@@ -305,6 +305,33 @@
     <t>Уровень: {level}
 Число волн: {wavecount}
 Следующий уровень: {nwavecount}
+Цена: {cost} камней.</t>
+  </si>
+  <si>
+    <t>shop_item_radar_desc</t>
+  </si>
+  <si>
+    <t>Allow detect UFO coord and direction
+Targets count equiv radar level</t>
+  </si>
+  <si>
+    <t>Позволяет определять позицию и
+направление НЛО. Число целей
+Равно уровню радара</t>
+  </si>
+  <si>
+    <t>shop_item_radar_tech</t>
+  </si>
+  <si>
+    <t>Level: {level}
+Target count: {targets}
+Next level: {ntargets}
+Cost: {cost} gems.</t>
+  </si>
+  <si>
+    <t>Уровень: {level}
+Число целей: {targets}
+Следующий уровень: {ntargets}
 Цена: {cost} камней.</t>
   </si>
 </sst>
@@ -410,17 +437,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.6122448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="37.3724489795918"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="48.9030612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.7040816326531"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="28.8979591836735"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -715,6 +742,28 @@
       </c>
       <c r="C27" s="2" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
gnum ready radar show grum (for free) resonator hit gnum & ufos teleport autorun the first wave of resonator fix typos
</commit_message>
<xml_diff>
--- a/Assets/excel/config.xlsx
+++ b/Assets/excel/config.xlsx
@@ -195,7 +195,7 @@
   <si>
     <t>Дополнительный корабль, который
 позволит продолжить игру после
-Гибели</t>
+гибели</t>
   </si>
   <si>
     <t>shop_item_ship_tech</t>
@@ -214,15 +214,16 @@
   <si>
     <t>Teleporter
 when key SPACEBAR pressed
-Then move ship at cursor pos instantly.
-After jump ship get 3sec invulnerability</t>
+Then move ship at cursor pos
+instantly. After jump ship get 3sec
+invulnerability</t>
   </si>
   <si>
     <t>Телепорт позволяет по нажатию
-кнопки ПРОБЕЛ переместиться в
-Точку положения прицела.
+кнопки ПРОБЕЛ переместиться
+в точку положения прицела.
 После прижка корабль получает
-Неузявимость на 3 секунды.</t>
+неузявимость на 3 секунды.</t>
   </si>
   <si>
     <t>shop_item_teleport_tech</t>
@@ -301,7 +302,8 @@
   </si>
   <si>
     <t>If press SPACEBAR inner 3 seconds
-after hyper jump appear wave that hit asteroids by 1 hp.</t>
+after hyper jump appear wave that hit
+asteroids by 1 hp.</t>
   </si>
   <si>
     <t>По выходу из гиперпространства
@@ -457,8 +459,8 @@
   </sheetPr>
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -674,7 +676,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
gnum forgoten assets main menu: add gnum, remove tutor button game: resize to smaller random bonus
</commit_message>
<xml_diff>
--- a/Assets/excel/config.xlsx
+++ b/Assets/excel/config.xlsx
@@ -62,13 +62,13 @@
     <t>Отключить звук</t>
   </si>
   <si>
-    <t>opt_disable_drag</t>
-  </si>
-  <si>
-    <t>Disable drag</t>
-  </si>
-  <si>
-    <t>Отключить трение</t>
+    <t>opt_drag</t>
+  </si>
+  <si>
+    <t>Drag</t>
+  </si>
+  <si>
+    <t>Трение</t>
   </si>
   <si>
     <t>opt_seamless_world</t>
@@ -459,8 +459,8 @@
   </sheetPr>
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
shop shotcut CTRL now
</commit_message>
<xml_diff>
--- a/Assets/excel/config.xlsx
+++ b/Assets/excel/config.xlsx
@@ -84,12 +84,12 @@
   </si>
   <si>
     <t>--- Keys ---
-ESC: shop (now all for free)
+CTRL: shop (now all for free)
 SPACE: teleport</t>
   </si>
   <si>
     <t>--- Клавиши ---
-ESC: магазин открыть/закрыть (все товары бесплатно)
+CTRL: магазин открыть/закрыть (все товары бесплатно)
 Пробел: телепорт</t>
   </si>
   <si>
@@ -460,7 +460,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>